<commit_message>
Alerts: added test case to check an archived FTP (attached) files
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1381,6 +1381,397 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>09.03.2022 13:53 (Kyiv+Israel) 10:53 (UTC) 19:53 (Japan) 16:23 (India)</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1.491</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-0.6780000000000002</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>09.04.2022 12:29 (Kyiv+Israel) 09:29 (UTC) 18:29 (Japan) 14:59 (India)</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1.282</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-0.4690000000000001</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>09.05.2022 09:06 (Kyiv+Israel) 06:06 (UTC) 15:06 (Japan) 11:36 (India)</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-0.272</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>09.05.2022 09:24 (Kyiv+Israel) 06:24 (UTC) 15:24 (Japan) 11:54 (India)</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>2.937</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-2.124</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>09.05.2022 12:16 (Kyiv+Israel) 09:16 (UTC) 18:16 (Japan) 14:46 (India)</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>2.489</v>
+      </c>
+      <c r="C44" t="n">
+        <v>-1.676</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>09.06.2022 10:31 (Kyiv+Israel) 07:31 (UTC) 16:31 (Japan) 13:01 (India)</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1.115</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-0.302</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>09.06.2022 18:44 (Kyiv+Israel) 15:44 (UTC) 00:44 (Japan) 21:14 (India)</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1.273</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-0.46</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>09.06.2022 21:26 (Kyiv+Israel) 18:26 (UTC) 03:26 (Japan) 23:56 (India)</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>3.514</v>
+      </c>
+      <c r="C47" t="n">
+        <v>-2.701</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>09.12.2022 09:26 (Kyiv+Israel) 06:26 (UTC) 15:26 (Japan) 11:56 (India)</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1.186</v>
+      </c>
+      <c r="C48" t="n">
+        <v>-0.373</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>09.12.2022 10:50 (Kyiv+Israel) 07:50 (UTC) 16:50 (Japan) 13:20 (India)</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>3.939</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-2.801</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:04 (Kyiv+Israel) 08:04 (UTC) 17:04 (Japan) 13:34 (India)</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="C50" t="n">
+        <v>-1.667</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:07 (Kyiv+Israel) 08:07 (UTC) 17:07 (Japan) 13:37 (India)</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>3.343</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-2.205</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:24 (Kyiv+Israel) 08:24 (UTC) 17:24 (Japan) 13:54 (India)</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>3.276</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-2.138</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:26 (Kyiv+Israel) 08:26 (UTC) 17:26 (Japan) 13:56 (India)</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>3.159</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-2.346</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:51 (Kyiv+Israel) 08:51 (UTC) 17:51 (Japan) 14:21 (India)</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>2.516</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-1.703</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>09.12.2022 12:09 (Kyiv+Israel) 09:09 (UTC) 18:09 (Japan) 14:39 (India)</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>3.217</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-2.404</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>09.14.2022 18:03 (Kyiv+Israel) 15:03 (UTC) 00:03 (Japan) 20:33 (India)</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1.661</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-0.5230000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1436,7 +1827,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -2390,6 +2781,420 @@
         </is>
       </c>
       <c r="E41" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>09.03.2022 13:50 (Kyiv+Israel) 10:50 (UTC) 19:50 (Japan) 16:20 (India)</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-0.1579999999999999</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>09.04.2022 12:26 (Kyiv+Israel) 09:26 (UTC) 18:26 (Japan) 14:56 (India)</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1.018</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-0.351</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>09.05.2022 09:03 (Kyiv+Israel) 06:03 (UTC) 15:03 (Japan) 11:33 (India)</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1.073</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>09.05.2022 09:21 (Kyiv+Israel) 06:21 (UTC) 15:21 (Japan) 11:51 (India)</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-0.128</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>09.05.2022 12:13 (Kyiv+Israel) 09:13 (UTC) 18:13 (Japan) 14:43 (India)</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.754</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-0.08699999999999997</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>09.05.2022 15:19 (Kyiv+Israel) 12:19 (UTC) 21:19 (Japan) 17:49 (India)</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.9429999999999999</v>
+      </c>
+      <c r="C47" t="n">
+        <v>-0.2759999999999999</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>09.06.2022 10:28 (Kyiv+Israel) 07:28 (UTC) 16:28 (Japan) 12:58 (India)</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="C48" t="n">
+        <v>-0.02099999999999991</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>09.06.2022 18:41 (Kyiv+Israel) 15:41 (UTC) 00:41 (Japan) 21:11 (India)</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.748</v>
+      </c>
+      <c r="C49" t="n">
+        <v>-0.08099999999999996</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>09.06.2022 21:23 (Kyiv+Israel) 18:23 (UTC) 03:23 (Japan) 23:53 (India)</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.908</v>
+      </c>
+      <c r="C50" t="n">
+        <v>-0.241</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>09.12.2022 09:03 (Kyiv+Israel) 06:03 (UTC) 15:03 (Japan) 11:33 (India)</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>1.257</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-0.3039999999999999</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>09.12.2022 09:22 (Kyiv+Israel) 06:22 (UTC) 15:22 (Japan) 11:52 (India)</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1.619</v>
+      </c>
+      <c r="C52" t="n">
+        <v>-0.952</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>09.12.2022 10:47 (Kyiv+Israel) 07:47 (UTC) 16:47 (Japan) 13:17 (India)</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>1.243</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-0.2900000000000001</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:00 (Kyiv+Israel) 08:00 (UTC) 17:00 (Japan) 13:30 (India)</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1.366</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-0.6990000000000001</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:04 (Kyiv+Israel) 08:04 (UTC) 17:04 (Japan) 13:34 (India)</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.927</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.02599999999999991</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:22 (Kyiv+Israel) 08:22 (UTC) 17:22 (Japan) 13:52 (India)</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1.132</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-0.2049999999999998</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:23 (Kyiv+Israel) 08:23 (UTC) 17:23 (Japan) 13:53 (India)</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-0.07299999999999995</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:48 (Kyiv+Israel) 08:48 (UTC) 17:48 (Japan) 14:18 (India)</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-0.203</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>09.12.2022 12:06 (Kyiv+Israel) 09:06 (UTC) 18:06 (Japan) 14:36 (India)</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1.079</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-0.4119999999999999</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -2482,7 +3287,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -3344,6 +4149,351 @@
         </is>
       </c>
       <c r="E37" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>09.03.2022 13:55 (Kyiv+Israel) 10:55 (UTC) 19:55 (Japan) 16:25 (India)</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>2.579</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-1.092</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>09.04.2022 12:31 (Kyiv+Israel) 09:31 (UTC) 18:31 (Japan) 15:01 (India)</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>2.586</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-1.099</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>09.05.2022 09:08 (Kyiv+Israel) 06:08 (UTC) 15:08 (Japan) 11:38 (India)</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>3.222</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-1.418</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>09.05.2022 12:19 (Kyiv+Israel) 09:19 (UTC) 18:19 (Japan) 14:49 (India)</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>2.184</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-0.6970000000000001</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>09.05.2022 15:24 (Kyiv+Israel) 12:24 (UTC) 21:24 (Japan) 17:54 (India)</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-1.303</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>09.06.2022 10:33 (Kyiv+Israel) 07:33 (UTC) 16:33 (Japan) 13:03 (India)</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>2.503</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-1.016</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>09.06.2022 18:46 (Kyiv+Israel) 15:46 (UTC) 00:46 (Japan) 21:16 (India)</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1.464</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.02300000000000013</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>09.06.2022 21:29 (Kyiv+Israel) 18:29 (UTC) 03:29 (Japan) 23:59 (India)</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>4.24</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-2.776</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>09.12.2022 10:54 (Kyiv+Israel) 07:54 (UTC) 16:54 (Japan) 13:24 (India)</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>4.702</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-2.898</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:07 (Kyiv+Israel) 08:07 (UTC) 17:07 (Japan) 13:37 (India)</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>3.686</v>
+      </c>
+      <c r="C47" t="n">
+        <v>-2.222</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:09 (Kyiv+Israel) 08:09 (UTC) 17:09 (Japan) 13:39 (India)</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-2.386</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:27 (Kyiv+Israel) 08:27 (UTC) 17:27 (Japan) 13:57 (India)</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>3.109</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-1.305</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:28 (Kyiv+Israel) 08:28 (UTC) 17:28 (Japan) 13:58 (India)</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>3.911</v>
+      </c>
+      <c r="C50" t="n">
+        <v>-2.447</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:54 (Kyiv+Israel) 08:54 (UTC) 17:54 (Japan) 14:24 (India)</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>3.656</v>
+      </c>
+      <c r="C51" t="n">
+        <v>-2.192</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>09.12.2022 12:12 (Kyiv+Israel) 09:12 (UTC) 18:12 (Japan) 14:42 (India)</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>4.241</v>
+      </c>
+      <c r="C52" t="n">
+        <v>-2.777</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -3436,7 +4586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -4275,6 +5425,305 @@
       </c>
       <c r="E36" t="n">
         <v>-0.38</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>09.03.2022 14:01 (Kyiv+Israel) 11:01 (UTC) 20:01 (Japan) 16:31 (India)</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-0.03900000000000003</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>09.05.2022 09:13 (Kyiv+Israel) 06:13 (UTC) 15:13 (Japan) 11:43 (India)</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1.209</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-0.287</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>09.05.2022 12:22 (Kyiv+Israel) 09:22 (UTC) 18:22 (Japan) 14:52 (India)</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.802</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-0.07600000000000007</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>09.05.2022 15:32 (Kyiv+Israel) 12:32 (UTC) 21:32 (Japan) 18:02 (India)</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.983</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-0.257</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>09.06.2022 10:41 (Kyiv+Israel) 07:41 (UTC) 16:41 (Japan) 13:11 (India)</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1.185</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-0.4590000000000001</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>09.06.2022 18:53 (Kyiv+Israel) 15:53 (UTC) 00:53 (Japan) 21:23 (India)</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.836</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>09.06.2022 21:36 (Kyiv+Israel) 18:36 (UTC) 03:36 (Japan) 00:06 (India)</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.761</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-0.03500000000000003</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>09.12.2022 10:58 (Kyiv+Israel) 07:58 (UTC) 16:58 (Japan) 13:28 (India)</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-0.5379999999999999</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:12 (Kyiv+Israel) 08:12 (UTC) 17:12 (Japan) 13:42 (India)</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-0.2679999999999999</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:15 (Kyiv+Israel) 08:15 (UTC) 17:15 (Japan) 13:45 (India)</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-0.104</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:29 (Kyiv+Israel) 08:29 (UTC) 17:29 (Japan) 13:59 (India)</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1.795</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-0.8729999999999999</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>09.12.2022 11:57 (Kyiv+Israel) 08:57 (UTC) 17:57 (Japan) 14:27 (India)</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.889</v>
+      </c>
+      <c r="C48" t="n">
+        <v>-0.163</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>09.12.2022 12:20 (Kyiv+Israel) 09:20 (UTC) 18:20 (Japan) 14:50 (India)</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1.762</v>
+      </c>
+      <c r="C49" t="n">
+        <v>-1.036</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fix for smoke tests
Minor fix for smoke tests (creation of row random number > 4)
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1772,6 +1772,213 @@
       </c>
       <c r="E56" t="n">
         <v>-0.5230000000000001</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>09.19.2022 09:39 (Kyiv+Israel) 06:39 (UTC) 15:39 (Japan) 12:09 (India)</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>5.369</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-4.556</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>09.19.2022 10:39 (Kyiv+Israel) 07:39 (UTC) 16:39 (Japan) 13:09 (India)</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>2.537</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-1.724</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>09.19.2022 10:43 (Kyiv+Israel) 07:43 (UTC) 16:43 (Japan) 13:13 (India)</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>2.918</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-1.78</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>09.19.2022 11:34 (Kyiv+Israel) 08:34 (UTC) 17:34 (Japan) 14:04 (India)</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2.356</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-1.218</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>09.19.2022 11:53 (Kyiv+Israel) 08:53 (UTC) 17:53 (Japan) 14:23 (India)</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>11.858</v>
+      </c>
+      <c r="C61" t="n">
+        <v>-11.045</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>09.19.2022 13:44 (Kyiv+Israel) 10:44 (UTC) 19:44 (Japan) 16:14 (India)</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1.246</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-0.4330000000000001</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>09.19.2022 13:47 (Kyiv+Israel) 10:47 (UTC) 19:47 (Japan) 16:17 (India)</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1.142</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-0.004000000000000004</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>09.19.2022 15:05 (Kyiv+Israel) 12:05 (UTC) 21:05 (Japan) 17:35 (India)</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1.456</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-0.643</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>09.19.2022 15:22 (Kyiv+Israel) 12:22 (UTC) 21:22 (Japan) 17:52 (India)</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1.595</v>
+      </c>
+      <c r="C65" t="n">
+        <v>-0.782</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1827,7 +2034,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -3195,6 +3402,144 @@
         </is>
       </c>
       <c r="E59" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>09.19.2022 09:42 (Kyiv+Israel) 06:42 (UTC) 15:42 (Japan) 12:12 (India)</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1.114</v>
+      </c>
+      <c r="C60" t="n">
+        <v>-0.4470000000000001</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>09.19.2022 09:45 (Kyiv+Israel) 06:45 (UTC) 15:45 (Japan) 12:15 (India)</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>1.903</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-0.976</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>09.19.2022 11:37 (Kyiv+Israel) 08:37 (UTC) 17:37 (Japan) 14:07 (India)</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1.091</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-0.1639999999999999</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>09.19.2022 11:56 (Kyiv+Israel) 08:56 (UTC) 17:56 (Japan) 14:26 (India)</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1.301</v>
+      </c>
+      <c r="C63" t="n">
+        <v>-0.6339999999999999</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>09.19.2022 15:07 (Kyiv+Israel) 12:07 (UTC) 21:07 (Japan) 17:37 (India)</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1.094</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-0.427</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>09.19.2022 15:25 (Kyiv+Israel) 12:25 (UTC) 21:25 (Japan) 17:55 (India)</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="C65" t="n">
+        <v>-0.08799999999999997</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -3287,7 +3632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -4494,6 +4839,144 @@
         </is>
       </c>
       <c r="E52" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>09.19.2022 09:44 (Kyiv+Israel) 06:44 (UTC) 15:44 (Japan) 12:14 (India)</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>3.236</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-1.772</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>09.19.2022 09:47 (Kyiv+Israel) 06:47 (UTC) 15:47 (Japan) 12:17 (India)</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>2.531</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.7270000000000001</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>09.19.2022 11:39 (Kyiv+Israel) 08:39 (UTC) 17:39 (Japan) 14:09 (India)</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>2.021</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0.2169999999999999</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>09.19.2022 11:59 (Kyiv+Israel) 08:59 (UTC) 17:59 (Japan) 14:29 (India)</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="C56" t="n">
+        <v>-0.7360000000000002</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>09.19.2022 15:10 (Kyiv+Israel) 12:10 (UTC) 21:10 (Japan) 17:40 (India)</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>3.657</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-2.193</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>09.19.2022 15:37 (Kyiv+Israel) 12:37 (UTC) 21:37 (Japan) 18:07 (India)</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-0.1759999999999999</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -4586,7 +5069,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -5721,6 +6204,144 @@
         </is>
       </c>
       <c r="E49" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>09.19.2022 09:49 (Kyiv+Israel) 06:49 (UTC) 15:49 (Japan) 12:19 (India)</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1.356</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-0.4340000000000001</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>09.19.2022 09:52 (Kyiv+Israel) 06:52 (UTC) 15:52 (Japan) 12:22 (India)</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>1.053</v>
+      </c>
+      <c r="C51" t="n">
+        <v>-0.327</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>09.19.2022 11:42 (Kyiv+Israel) 08:42 (UTC) 17:42 (Japan) 14:12 (India)</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1.274</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-0.352</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>09.19.2022 12:09 (Kyiv+Israel) 09:09 (UTC) 18:09 (Japan) 14:39 (India)</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1.242</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-0.516</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>09.19.2022 15:18 (Kyiv+Israel) 12:18 (UTC) 21:18 (Japan) 17:48 (India)</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.736</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-0.01000000000000001</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>09.19.2022 15:40 (Kyiv+Israel) 12:40 (UTC) 21:40 (Japan) 18:10 (India)</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.836</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
         <is>
           <t>***</t>
         </is>

</xml_diff>

<commit_message>
Added page load validation
Added page load validation (test will fails if > 25 sec)
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1976,6 +1976,98 @@
         </is>
       </c>
       <c r="E65" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>09.19.2022 16:17 (Kyiv+Israel) 13:17 (UTC) 22:17 (Japan) 18:47 (India)</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.912</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-0.09900000000000009</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>09.21.2022 09:39 (Kyiv+Israel) 06:39 (UTC) 15:39 (Japan) 12:09 (India)</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>1.644</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-0.506</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>09.26.2022 09:05 (Kyiv+Israel) 06:05 (UTC) 15:05 (Japan) 11:35 (India)</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-0.06200000000000006</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>09.27.2022 09:33 (Kyiv+Israel) 06:33 (UTC) 15:33 (Japan) 12:03 (India)</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="C69" t="n">
+        <v>-1.367</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -2034,7 +2126,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -3540,6 +3632,98 @@
         </is>
       </c>
       <c r="E65" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>09.19.2022 16:19 (Kyiv+Israel) 13:19 (UTC) 22:19 (Japan) 18:49 (India)</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1.022</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-0.355</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>09.21.2022 09:42 (Kyiv+Israel) 06:42 (UTC) 15:42 (Japan) 12:12 (India)</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.9370000000000001</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-0.01000000000000001</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>09.26.2022 09:09 (Kyiv+Israel) 06:09 (UTC) 15:09 (Japan) 11:39 (India)</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.162</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>09.27.2022 09:35 (Kyiv+Israel) 06:35 (UTC) 15:35 (Japan) 12:05 (India)</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.631</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.03600000000000003</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -3632,7 +3816,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -4977,6 +5161,98 @@
         </is>
       </c>
       <c r="E58" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>09.19.2022 16:22 (Kyiv+Israel) 13:22 (UTC) 22:22 (Japan) 18:52 (India)</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>2.754</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-1.29</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>09.21.2022 09:44 (Kyiv+Israel) 06:44 (UTC) 15:44 (Japan) 12:14 (India)</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2.011</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-0.2070000000000001</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>09.26.2022 09:12 (Kyiv+Israel) 06:12 (UTC) 15:12 (Japan) 11:42 (India)</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>1.966</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-0.1619999999999999</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>09.27.2022 09:38 (Kyiv+Israel) 06:38 (UTC) 15:38 (Japan) 12:08 (India)</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>2.656</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-1.192</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -5069,7 +5345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -6342,6 +6618,213 @@
         </is>
       </c>
       <c r="E55" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>09.19.2022 16:30 (Kyiv+Israel) 13:30 (UTC) 22:30 (Japan) 19:00 (India)</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.828</v>
+      </c>
+      <c r="C56" t="n">
+        <v>-0.102</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>09.21.2022 09:32 (Kyiv+Israel) 06:32 (UTC) 15:32 (Japan) 12:02 (India)</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1.243</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-0.5170000000000001</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>09.21.2022 09:47 (Kyiv+Israel) 06:47 (UTC) 15:47 (Japan) 12:17 (India)</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>1.256</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-0.334</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>09.22.2022 18:26 (Kyiv+Israel) 15:26 (UTC) 00:26 (Japan) 20:56 (India)</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.873</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-0.147</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>09.24.2022 20:55 (Kyiv+Israel) 17:55 (UTC) 02:55 (Japan) 23:25 (India)</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="C60" t="n">
+        <v>-0.08400000000000007</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>09.26.2022 09:15 (Kyiv+Israel) 06:15 (UTC) 15:15 (Japan) 11:45 (India)</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>1.096</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-0.174</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>09.26.2022 09:52 (Kyiv+Israel) 06:52 (UTC) 15:52 (Japan) 12:22 (India)</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.869</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-0.143</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>09.26.2022 17:11 (Kyiv+Israel) 14:11 (UTC) 23:11 (Japan) 19:41 (India)</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.747</v>
+      </c>
+      <c r="C63" t="n">
+        <v>-0.02100000000000002</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>09.27.2022 09:44 (Kyiv+Israel) 06:44 (UTC) 15:44 (Japan) 12:14 (India)</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.8139999999999999</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-0.08799999999999997</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
         <is>
           <t>***</t>
         </is>

</xml_diff>

<commit_message>
Added test case for Notion bug: Order becomes expired, unassigned if changing date from Manual assignment
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2275,6 +2275,75 @@
         </is>
       </c>
       <c r="E78" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>10.07.2022 16:44 (Kyiv+Israel) 13:44 (UTC) 22:44 (Japan) 19:14 (India)</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.802</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-0.07500000000000007</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>10.10.2022 09:04 (Kyiv+Israel) 06:04 (UTC) 15:04 (Japan) 11:34 (India)</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-0.7370000000000001</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>10.10.2022 09:21 (Kyiv+Israel) 06:21 (UTC) 15:21 (Japan) 11:51 (India)</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-0.144</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -2333,7 +2402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -4023,6 +4092,75 @@
         </is>
       </c>
       <c r="E73" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>10.07.2022 16:47 (Kyiv+Israel) 13:47 (UTC) 22:47 (Japan) 19:17 (India)</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.637</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-0.006000000000000005</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>10.10.2022 09:08 (Kyiv+Israel) 06:08 (UTC) 15:08 (Japan) 11:38 (India)</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.896</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-0.131</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>10.10.2022 09:26 (Kyiv+Israel) 06:26 (UTC) 15:26 (Japan) 11:56 (India)</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1.103</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-0.472</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -4115,7 +4253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -5624,6 +5762,121 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>10.07.2022 16:50 (Kyiv+Israel) 13:50 (UTC) 22:50 (Japan) 19:20 (India)</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>2.278</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-0.8140000000000001</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>10.10.2022 09:11 (Kyiv+Israel) 06:11 (UTC) 15:11 (Japan) 11:41 (India)</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>1.584</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>10.10.2022 09:29 (Kyiv+Israel) 06:29 (UTC) 15:29 (Japan) 11:59 (India)</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1.104</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.3599999999999999</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>10.11.2022 23:02 (Kyiv+Israel) 20:02 (UTC) 05:02 (Japan) 01:32 (India)</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1.231</v>
+      </c>
+      <c r="C69" t="n">
+        <v>-0.127</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>10.11.2022 23:04 (Kyiv+Israel) 20:04 (UTC) 05:04 (Japan) 01:34 (India)</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.3159999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -5713,7 +5966,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -7446,6 +7699,75 @@
         </is>
       </c>
       <c r="E75" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>10.07.2022 16:57 (Kyiv+Israel) 13:57 (UTC) 22:57 (Japan) 19:27 (India)</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.768</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-0.103</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>10.10.2022 09:13 (Kyiv+Israel) 06:13 (UTC) 15:13 (Japan) 11:43 (India)</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.9409999999999999</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-0.01899999999999991</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>10.10.2022 09:35 (Kyiv+Israel) 06:35 (UTC) 15:35 (Japan) 12:05 (India)</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.6860000000000001</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-0.02100000000000002</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
         <is>
           <t>***</t>
         </is>

</xml_diff>

<commit_message>
Added whats app B
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2347,6 +2347,29 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>10.13.2022 12:51 (Kyiv+Israel) 09:51 (UTC) 18:51 (Japan) 15:21 (India)</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-0.4870000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -4164,6 +4187,29 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>10.13.2022 12:40 (Kyiv+Israel) 09:40 (UTC) 18:40 (Japan) 15:10 (India)</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.967</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-0.202</v>
       </c>
     </row>
   </sheetData>
@@ -4253,7 +4299,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -5877,6 +5923,52 @@
       </c>
       <c r="E70" t="n">
         <v>-0.3159999999999998</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>10.13.2022 12:53 (Kyiv+Israel) 09:53 (UTC) 18:53 (Japan) 15:23 (India)</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-0.9159999999999999</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>10.13.2022 14:43 (Kyiv+Israel) 11:43 (UTC) 20:43 (Japan) 17:13 (India)</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>2.041</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-0.4569999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -5966,7 +6058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -7771,6 +7863,98 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>10.12.2022 10:48 (Kyiv+Israel) 07:48 (UTC) 16:48 (Japan) 13:18 (India)</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-0.3079999999999999</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>10.12.2022 10:50 (Kyiv+Israel) 07:50 (UTC) 16:50 (Japan) 13:20 (India)</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.979</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-0.05699999999999994</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>10.13.2022 13:14 (Kyiv+Israel) 10:14 (UTC) 19:14 (Japan) 15:44 (India)</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>1.081</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-0.1589999999999999</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>10.13.2022 14:40 (Kyiv+Israel) 11:40 (UTC) 20:40 (Japan) 17:10 (India)</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>1.222</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-0.2999999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for certification case
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -6058,7 +6058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -7955,6 +7955,121 @@
       </c>
       <c r="E82" t="n">
         <v>-0.2999999999999999</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>10.13.2022 17:58 (Kyiv+Israel) 14:58 (UTC) 23:58 (Japan) 20:28 (India)</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>1.024</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-0.102</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>10.13.2022 18:01 (Kyiv+Israel) 15:01 (UTC) 00:01 (Japan) 20:31 (India)</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>1.672</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-0.7499999999999999</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>10.13.2022 18:13 (Kyiv+Israel) 15:13 (UTC) 00:13 (Japan) 20:43 (India)</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>1.001</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-0.07899999999999985</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10.13.2022 18:30 (Kyiv+Israel) 15:30 (UTC) 00:30 (Japan) 21:00 (India)</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>1.106</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-0.1840000000000001</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>10.13.2022 18:33 (Kyiv+Israel) 15:33 (UTC) 00:33 (Japan) 21:03 (India)</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-0.269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix for auth page
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2370,6 +2370,29 @@
       </c>
       <c r="E82" t="n">
         <v>-0.4870000000000001</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>10.13.2022 18:52 (Kyiv+Israel) 15:52 (UTC) 00:52 (Japan) 21:22 (India)</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>1.433</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-0.2950000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -2425,7 +2448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -4210,6 +4233,29 @@
       </c>
       <c r="E77" t="n">
         <v>-0.202</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>10.13.2022 18:54 (Kyiv+Israel) 15:54 (UTC) 00:54 (Japan) 21:24 (India)</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.593</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.172</v>
       </c>
     </row>
   </sheetData>
@@ -4299,7 +4345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -5969,6 +6015,29 @@
       </c>
       <c r="E72" t="n">
         <v>-0.4569999999999999</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>10.13.2022 18:57 (Kyiv+Israel) 15:57 (UTC) 00:57 (Japan) 21:27 (India)</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>1.917</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-0.333</v>
       </c>
     </row>
   </sheetData>
@@ -6058,7 +6127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -8070,6 +8139,52 @@
       </c>
       <c r="E87" t="n">
         <v>-0.269</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>10.13.2022 18:59 (Kyiv+Israel) 15:59 (UTC) 00:59 (Japan) 21:29 (India)</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-0.07399999999999995</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>10.13.2022 19:23 (Kyiv+Israel) 16:23 (UTC) 01:23 (Japan) 21:53 (India)</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="C89" t="n">
+        <v>-0.06999999999999995</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test for WhatsApp
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2393,6 +2393,52 @@
       </c>
       <c r="E83" t="n">
         <v>-0.2950000000000002</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>10.13.2022 19:46 (Kyiv+Israel) 16:46 (UTC) 01:46 (Japan) 22:16 (India)</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>1.586</v>
+      </c>
+      <c r="C84" t="n">
+        <v>-0.8590000000000001</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>10.13.2022 20:06 (Kyiv+Israel) 17:06 (UTC) 02:06 (Japan) 22:36 (India)</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0.802</v>
+      </c>
+      <c r="C85" t="n">
+        <v>-0.07500000000000007</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -2448,7 +2494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -4256,6 +4302,52 @@
       </c>
       <c r="E78" t="n">
         <v>0.172</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>10.13.2022 19:49 (Kyiv+Israel) 16:49 (UTC) 01:49 (Japan) 22:19 (India)</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-0.03300000000000003</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>10.13.2022 20:09 (Kyiv+Israel) 17:09 (UTC) 02:09 (Japan) 22:39 (India)</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.881</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -4345,7 +4437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -6038,6 +6130,52 @@
       </c>
       <c r="E73" t="n">
         <v>-0.333</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>10.13.2022 19:51 (Kyiv+Israel) 16:51 (UTC) 01:51 (Japan) 22:21 (India)</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>1.356</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-0.252</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>10.13.2022 20:11 (Kyiv+Israel) 17:11 (UTC) 02:11 (Japan) 22:41 (India)</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1.406</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-0.3019999999999998</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -6127,7 +6265,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -8182,6 +8320,29 @@
         </is>
       </c>
       <c r="E89" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>10.13.2022 20:14 (Kyiv+Israel) 17:14 (UTC) 02:14 (Japan) 22:44 (India)</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0.754</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-0.08899999999999997</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
         <is>
           <t>***</t>
         </is>

</xml_diff>

<commit_message>
Added test to check SMS and Email surveys (creation/update/send invitation)
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2439,6 +2439,52 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10.17.2022 12:54 (Kyiv+Israel) 09:54 (UTC) 18:54 (Japan) 15:24 (India)</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>1.487</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-0.7600000000000001</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>10.17.2022 12:59 (Kyiv+Israel) 09:59 (UTC) 18:59 (Japan) 15:29 (India)</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>2.849</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-1.711</v>
       </c>
     </row>
   </sheetData>
@@ -4437,7 +4483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -6173,6 +6219,29 @@
         </is>
       </c>
       <c r="E75" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>10.20.2022 23:26 (Kyiv+Israel) 20:26 (UTC) 05:26 (Japan) 01:56 (India)</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1.707</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-0.603</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -6265,7 +6334,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -8343,6 +8412,29 @@
         </is>
       </c>
       <c r="E90" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>10.20.2022 23:35 (Kyiv+Israel) 20:35 (UTC) 05:35 (Japan) 02:05 (India)</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.849</v>
+      </c>
+      <c r="C91" t="n">
+        <v>-0.1839999999999999</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
         <is>
           <t>***</t>
         </is>

</xml_diff>

<commit_message>
Minor fix for sample upload issue
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2485,6 +2485,75 @@
       </c>
       <c r="E87" t="n">
         <v>-1.711</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>10.21.2022 10:20 (Kyiv+Israel) 07:20 (UTC) 16:20 (Japan) 12:50 (India)</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>1.583</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-0.856</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>10.21.2022 15:04 (Kyiv+Israel) 12:04 (UTC) 21:04 (Japan) 17:34 (India)</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0.862</v>
+      </c>
+      <c r="C89" t="n">
+        <v>-0.135</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>10.24.2022 13:03 (Kyiv+Israel) 10:03 (UTC) 19:03 (Japan) 15:33 (India)</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-0.293</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -2540,7 +2609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -4391,6 +4460,75 @@
         </is>
       </c>
       <c r="E80" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>10.21.2022 11:15 (Kyiv+Israel) 08:15 (UTC) 17:15 (Japan) 13:45 (India)</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-0.104</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>10.21.2022 15:07 (Kyiv+Israel) 12:07 (UTC) 21:07 (Japan) 17:37 (India)</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="C82" t="n">
+        <v>-0.284</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>10.24.2022 13:06 (Kyiv+Israel) 10:06 (UTC) 19:06 (Japan) 15:36 (India)</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>1.501</v>
+      </c>
+      <c r="C83" t="n">
+        <v>-0.8699999999999999</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -4483,7 +4621,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -6242,6 +6380,121 @@
         </is>
       </c>
       <c r="E76" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>10.21.2022 11:29 (Kyiv+Israel) 08:29 (UTC) 17:29 (Japan) 13:59 (India)</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>1.741</v>
+      </c>
+      <c r="C77" t="n">
+        <v>-0.637</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>10.21.2022 11:55 (Kyiv+Israel) 08:55 (UTC) 17:55 (Japan) 14:25 (India)</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-0.5559999999999998</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>10.21.2022 14:29 (Kyiv+Israel) 11:29 (UTC) 20:29 (Japan) 16:59 (India)</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-0.3159999999999998</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>10.21.2022 15:10 (Kyiv+Israel) 12:10 (UTC) 21:10 (Japan) 17:40 (India)</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>1.637</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-0.5329999999999999</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>10.24.2022 13:48 (Kyiv+Israel) 10:48 (UTC) 19:48 (Japan) 16:18 (India)</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>2.375</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-1.271</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -6334,7 +6587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -8435,6 +8688,75 @@
         </is>
       </c>
       <c r="E91" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>10.21.2022 11:24 (Kyiv+Israel) 08:24 (UTC) 17:24 (Japan) 13:54 (India)</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0.878</v>
+      </c>
+      <c r="C92" t="n">
+        <v>-0.213</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>10.21.2022 15:19 (Kyiv+Israel) 12:19 (UTC) 21:19 (Japan) 17:49 (India)</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>1.202</v>
+      </c>
+      <c r="C93" t="n">
+        <v>-0.5369999999999999</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>10.24.2022 13:53 (Kyiv+Israel) 10:53 (UTC) 19:53 (Japan) 16:23 (India)</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="C94" t="n">
+        <v>-0.4949999999999999</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
         <is>
           <t>***</t>
         </is>

</xml_diff>

<commit_message>
Added test for SAMPLE AUTO IMPORT
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2551,6 +2551,29 @@
         </is>
       </c>
       <c r="E90" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>10.28.2022 21:49 (Kyiv+Israel) 18:49 (UTC) 03:49 (Japan) 00:19 (India)</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="C91" t="n">
+        <v>-0.108</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -2609,7 +2632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -4529,6 +4552,144 @@
         </is>
       </c>
       <c r="E83" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>10.28.2022 13:00 (Kyiv+Israel) 10:00 (UTC) 19:00 (Japan) 15:30 (India)</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>1.023</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-0.4299999999999999</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>10.28.2022 13:03 (Kyiv+Israel) 10:03 (UTC) 19:03 (Japan) 15:33 (India)</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>1.104</v>
+      </c>
+      <c r="C85" t="n">
+        <v>-0.4730000000000001</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10.28.2022 13:06 (Kyiv+Israel) 10:06 (UTC) 19:06 (Japan) 15:36 (India)</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-0.01200000000000001</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>10.28.2022 13:21 (Kyiv+Israel) 10:21 (UTC) 19:21 (Japan) 15:51 (India)</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0.979</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-0.348</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>10.28.2022 21:06 (Kyiv+Israel) 18:06 (UTC) 03:06 (Japan) 23:36 (India)</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>0.716</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-0.08499999999999996</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>10.28.2022 21:52 (Kyiv+Israel) 18:52 (UTC) 03:52 (Japan) 00:22 (India)</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.05100000000000005</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -4621,7 +4782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -6495,6 +6656,29 @@
         </is>
       </c>
       <c r="E81" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>10.28.2022 21:54 (Kyiv+Israel) 18:54 (UTC) 03:54 (Japan) 00:24 (India)</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>1.398</v>
+      </c>
+      <c r="C82" t="n">
+        <v>-0.2939999999999998</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -6587,7 +6771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -8757,6 +8941,29 @@
         </is>
       </c>
       <c r="E94" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>10.28.2022 22:02 (Kyiv+Israel) 19:02 (UTC) 04:02 (Japan) 00:32 (India)</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="C95" t="n">
+        <v>-0.06799999999999995</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
         <is>
           <t>***</t>
         </is>

</xml_diff>

<commit_message>
Addeв case for creation Bank and its Branches
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2574,6 +2574,144 @@
         </is>
       </c>
       <c r="E91" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>11.01.2022 17:23 (Kyiv+Israel) 15:23 (UTC) 00:23 (Japan) 20:53 (India)</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>6.476</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-5.338</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>11.01.2022 18:01 (Kyiv+Israel) 16:01 (UTC) 01:01 (Japan) 21:31 (India)</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>3.201</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-2.063</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>11.02.2022 13:46 (Kyiv+Israel) 11:46 (UTC) 20:46 (Japan) 17:16 (India)</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-2.743</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>11.02.2022 14:38 (Kyiv+Israel) 12:38 (UTC) 21:38 (Japan) 18:08 (India)</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>4.187</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-3.049</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>11.07.2022 11:08 (Kyiv+Israel) 09:08 (UTC) 18:08 (Japan) 14:38 (India)</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>2.116</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-0.9780000000000002</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>11.07.2022 11:10 (Kyiv+Israel) 09:10 (UTC) 18:10 (Japan) 14:40 (India)</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>1.807</v>
+      </c>
+      <c r="C97" t="n">
+        <v>-1.08</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -2632,7 +2770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -4690,6 +4828,144 @@
         </is>
       </c>
       <c r="E89" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>11.01.2022 17:33 (Kyiv+Israel) 15:33 (UTC) 00:33 (Japan) 21:03 (India)</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>1.222</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-0.629</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>11.01.2022 18:04 (Kyiv+Israel) 16:04 (UTC) 01:04 (Japan) 21:34 (India)</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>3.854</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-3.261</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>11.02.2022 13:49 (Kyiv+Israel) 11:49 (UTC) 20:49 (Japan) 17:19 (India)</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.772</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-0.179</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>11.02.2022 14:41 (Kyiv+Israel) 12:41 (UTC) 21:41 (Japan) 18:11 (India)</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>1.356</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-0.7630000000000001</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>11.07.2022 11:12 (Kyiv+Israel) 09:12 (UTC) 18:12 (Japan) 14:42 (India)</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.958</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-0.365</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>11.07.2022 11:13 (Kyiv+Israel) 09:13 (UTC) 18:13 (Japan) 14:43 (India)</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="C95" t="n">
+        <v>-0.245</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -4782,7 +5058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -6679,6 +6955,121 @@
         </is>
       </c>
       <c r="E82" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>11.01.2022 18:07 (Kyiv+Israel) 16:07 (UTC) 01:07 (Japan) 21:37 (India)</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>3.305</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-1.721</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>11.02.2022 13:52 (Kyiv+Israel) 11:52 (UTC) 20:52 (Japan) 17:22 (India)</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>4.095</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-2.511</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>11.02.2022 14:43 (Kyiv+Israel) 12:43 (UTC) 21:43 (Japan) 18:13 (India)</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>6.016</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-4.432</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>11.07.2022 11:14 (Kyiv+Israel) 09:14 (UTC) 18:14 (Japan) 14:44 (India)</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>1.585</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-0.0009999999999998899</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>11.07.2022 11:16 (Kyiv+Israel) 09:16 (UTC) 18:16 (Japan) 14:46 (India)</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>2.066</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-0.9619999999999997</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -6771,7 +7162,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -8964,6 +9355,98 @@
         </is>
       </c>
       <c r="E95" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>11.02.2022 13:41 (Kyiv+Israel) 11:41 (UTC) 20:41 (Japan) 17:11 (India)</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>3.199</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-2.277</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>11.02.2022 14:47 (Kyiv+Israel) 12:47 (UTC) 21:47 (Japan) 18:17 (India)</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>1.434</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-0.5119999999999999</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>11.07.2022 11:17 (Kyiv+Israel) 09:17 (UTC) 18:17 (Japan) 14:47 (India)</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-0.108</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>11.07.2022 11:24 (Kyiv+Israel) 09:24 (UTC) 18:24 (Japan) 14:54 (India)</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="C99" t="n">
+        <v>-0.3069999999999999</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
         <is>
           <t>***</t>
         </is>

</xml_diff>

<commit_message>
fix for succ message (adding sample row)
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2804,6 +2804,144 @@
         </is>
       </c>
       <c r="E101" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>11.28.2022 12:03 (Kyiv+Israel) 10:03 (UTC) 19:03 (Japan) 15:33 (India)</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="C102" t="n">
+        <v>-0.246</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>12.05.2022 09:21 (Kyiv+Israel) 07:21 (UTC) 16:21 (Japan) 12:51 (India)</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>2.624</v>
+      </c>
+      <c r="C103" t="n">
+        <v>-1.897</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>12.05.2022 10:22 (Kyiv+Israel) 08:22 (UTC) 17:22 (Japan) 13:52 (India)</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>1.808</v>
+      </c>
+      <c r="C104" t="n">
+        <v>-1.081</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>12.05.2022 11:29 (Kyiv+Israel) 09:29 (UTC) 18:29 (Japan) 14:59 (India)</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>3.131</v>
+      </c>
+      <c r="C105" t="n">
+        <v>-2.404</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>12.05.2022 17:14 (Kyiv+Israel) 15:14 (UTC) 00:14 (Japan) 20:44 (India)</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>1.843</v>
+      </c>
+      <c r="E106" t="n">
+        <v>-0.7050000000000001</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>12.05.2022 17:15 (Kyiv+Israel) 15:15 (UTC) 00:15 (Japan) 20:45 (India)</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>2.408</v>
+      </c>
+      <c r="C107" t="n">
+        <v>-1.681</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -2862,7 +3000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -5150,6 +5288,144 @@
         </is>
       </c>
       <c r="E99" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>12.05.2022 09:09 (Kyiv+Israel) 07:09 (UTC) 16:09 (Japan) 12:39 (India)</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-0.405</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>12.05.2022 09:24 (Kyiv+Israel) 07:24 (UTC) 16:24 (Japan) 12:54 (India)</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0.983</v>
+      </c>
+      <c r="C101" t="n">
+        <v>-0.403</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>12.05.2022 10:24 (Kyiv+Israel) 08:24 (UTC) 17:24 (Japan) 13:54 (India)</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0.9389999999999999</v>
+      </c>
+      <c r="C102" t="n">
+        <v>-0.359</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>12.05.2022 11:32 (Kyiv+Israel) 09:32 (UTC) 18:32 (Japan) 15:02 (India)</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>1.162</v>
+      </c>
+      <c r="C103" t="n">
+        <v>-0.582</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>12.05.2022 17:18 (Kyiv+Israel) 15:18 (UTC) 00:18 (Japan) 20:48 (India)</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>1.371</v>
+      </c>
+      <c r="E104" t="n">
+        <v>-0.778</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>12.05.2022 17:19 (Kyiv+Israel) 15:19 (UTC) 00:19 (Japan) 20:49 (India)</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>1.408</v>
+      </c>
+      <c r="C105" t="n">
+        <v>-0.828</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -5242,7 +5518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -7349,6 +7625,144 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>12.05.2022 10:09 (Kyiv+Israel) 08:09 (UTC) 17:09 (Japan) 13:39 (India)</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>3.086</v>
+      </c>
+      <c r="C92" t="n">
+        <v>-1.982</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>12.05.2022 10:27 (Kyiv+Israel) 08:27 (UTC) 17:27 (Japan) 13:57 (India)</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="C93" t="n">
+        <v>-1.696</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>12.05.2022 17:22 (Kyiv+Israel) 15:22 (UTC) 00:22 (Japan) 20:52 (India)</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>8.101000000000001</v>
+      </c>
+      <c r="C94" t="n">
+        <v>-6.997000000000001</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>12.05.2022 23:30 (Kyiv+Israel) 21:30 (UTC) 06:30 (Japan) 03:00 (India)</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>2.945</v>
+      </c>
+      <c r="C95" t="n">
+        <v>-1.841</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>12.05.2022 23:40 (Kyiv+Israel) 21:40 (UTC) 06:40 (Japan) 03:10 (India)</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>1.833</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-0.2489999999999999</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>12.05.2022 23:46 (Kyiv+Israel) 21:46 (UTC) 06:46 (Japan) 03:16 (India)</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>1.666</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-0.08199999999999985</v>
       </c>
     </row>
   </sheetData>
@@ -7438,7 +7852,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -9815,6 +10229,144 @@
         </is>
       </c>
       <c r="E103" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>12.05.2022 09:53 (Kyiv+Israel) 07:53 (UTC) 16:53 (Japan) 13:23 (India)</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0.831</v>
+      </c>
+      <c r="C104" t="n">
+        <v>-0.1659999999999999</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>12.05.2022 09:55 (Kyiv+Israel) 07:55 (UTC) 16:55 (Japan) 13:25 (India)</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>1.211</v>
+      </c>
+      <c r="E105" t="n">
+        <v>-0.289</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>12.05.2022 10:17 (Kyiv+Israel) 08:17 (UTC) 17:17 (Japan) 13:47 (India)</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>1.025</v>
+      </c>
+      <c r="C106" t="n">
+        <v>-0.3599999999999999</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>12.05.2022 11:39 (Kyiv+Israel) 09:39 (UTC) 18:39 (Japan) 15:09 (India)</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>0.974</v>
+      </c>
+      <c r="C107" t="n">
+        <v>-0.3089999999999999</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>12.05.2022 17:24 (Kyiv+Israel) 15:24 (UTC) 00:24 (Japan) 20:54 (India)</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>1.233</v>
+      </c>
+      <c r="E108" t="n">
+        <v>-0.3110000000000001</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>12.05.2022 17:32 (Kyiv+Israel) 15:32 (UTC) 00:32 (Japan) 21:02 (India)</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>0.889</v>
+      </c>
+      <c r="C109" t="n">
+        <v>-0.224</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
         <is>
           <t>***</t>
         </is>

</xml_diff>

<commit_message>
[Email Survey] Added validation for email body, subject and link
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -2945,6 +2945,29 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>12.06.2022 00:45 (Kyiv+Israel) 22:45 (UTC) 07:45 (Japan) 04:15 (India)</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>0.993</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.1449999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3000,7 +3023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -5429,6 +5452,29 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>12.06.2022 00:48 (Kyiv+Israel) 22:48 (UTC) 07:48 (Japan) 04:18 (India)</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.003000000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -5518,7 +5564,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A3:E21"/>
@@ -7763,6 +7809,29 @@
       </c>
       <c r="E97" t="n">
         <v>-0.08199999999999985</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>12.06.2022 00:50 (Kyiv+Israel) 22:50 (UTC) 07:50 (Japan) 04:20 (India)</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>1.505</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.07900000000000018</v>
       </c>
     </row>
   </sheetData>
@@ -7852,7 +7921,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -10370,6 +10439,29 @@
         <is>
           <t>***</t>
         </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>12.06.2022 00:53 (Kyiv+Israel) 22:53 (UTC) 07:53 (Japan) 04:23 (India)</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>1.015</v>
+      </c>
+      <c r="E110" t="n">
+        <v>-0.09299999999999986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for order time [MystShopping]
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E110"/>
@@ -528,113 +528,171 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>12.16.2022 19:21 (Kyiv+Israel) 17:21 (UTC) 02:21 (Japan) 22:51 (India)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.217</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>12.16.2022 19:26 (Kyiv+Israel) 17:26 (UTC) 02:26 (Japan) 22:56 (India)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.094</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>12.19.2022 14:25 (Kyiv+Israel) 12:25 (UTC) 21:25 (Japan) 17:55 (India)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1.341</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.2469999999999999</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12.19.2022 15:53 (Kyiv+Israel) 13:53 (UTC) 22:53 (Japan) 19:23 (India)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1.135</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12.19.2022 16:09 (Kyiv+Israel) 14:09 (UTC) 23:09 (Japan) 19:39 (India)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2.638</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1.503</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>12.19.2022 16:21 (Kyiv+Israel) 14:21 (UTC) 23:21 (Japan) 19:51 (India)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.466</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-0.3719999999999999</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>12.21.2022 01:53 (Kyiv+Israel) 23:53 (UTC) 08:53 (Japan) 05:23 (India)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1.604</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.51</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
@@ -688,7 +746,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F261"/>
@@ -746,112 +804,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
@@ -872,6 +824,146 @@
         </is>
       </c>
       <c r="E109" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>12.19.2022 14:28 (Kyiv+Israel) 12:28 (UTC) 21:28 (Japan) 17:58 (India)</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>1.247</v>
+      </c>
+      <c r="C110" t="n">
+        <v>-0.4870000000000001</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>12.19.2022 14:42 (Kyiv+Israel) 12:42 (UTC) 21:42 (Japan) 18:12 (India)</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>1.237</v>
+      </c>
+      <c r="C111" t="n">
+        <v>-0.4770000000000001</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>12.19.2022 15:56 (Kyiv+Israel) 13:56 (UTC) 22:56 (Japan) 19:26 (India)</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>0.905</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>12.19.2022 16:11 (Kyiv+Israel) 14:11 (UTC) 23:11 (Japan) 19:41 (India)</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>0.654</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.251</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>12.19.2022 16:24 (Kyiv+Israel) 14:24 (UTC) 23:24 (Japan) 19:54 (India)</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>1.038</v>
+      </c>
+      <c r="C114" t="n">
+        <v>-0.278</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>12.21.2022 01:06 (Kyiv+Israel) 23:06 (UTC) 08:06 (Japan) 04:36 (India)</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>0.642</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.118</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -964,7 +1056,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F101"/>
@@ -1022,104 +1114,125 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>12.19.2022 14:31 (Kyiv+Israel) 12:31 (UTC) 21:31 (Japan) 18:01 (India)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2.643</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>12.19.2022 15:58 (Kyiv+Israel) 13:58 (UTC) 22:58 (Japan) 19:28 (India)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1.735</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>12.19.2022 16:14 (Kyiv+Israel) 14:14 (UTC) 23:14 (Japan) 19:44 (India)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1.646</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.08900000000000019</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12.19.2022 16:27 (Kyiv+Israel) 14:27 (UTC) 23:27 (Japan) 19:57 (India)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2.732</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.08900000000000041</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12.21.2022 01:09 (Kyiv+Israel) 23:09 (UTC) 08:09 (Japan) 04:39 (India)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.108</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5349999999999997</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
@@ -1207,7 +1320,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F113"/>
@@ -1262,115 +1375,102 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>12.19.2022 14:46 (Kyiv+Israel) 12:46 (UTC) 21:46 (Japan) 18:16 (India)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.152</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>12.19.2022 16:11 (Kyiv+Israel) 14:11 (UTC) 23:11 (Japan) 19:41 (India)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1.127</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>12.19.2022 16:17 (Kyiv+Israel) 14:17 (UTC) 23:17 (Japan) 19:47 (India)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2.332</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1.205</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12.21.2022 01:26 (Kyiv+Israel) 23:26 (UTC) 08:26 (Japan) 04:56 (India)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.806</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.3459999999999999</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
Fix for smoke test (Jenkins server)
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -1504,7 +1504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F113"/>
@@ -1724,6 +1724,52 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01.07.2023 00:15 (Kyiv+Israel) 22:15 (UTC) 07:15 (Japan) 03:45 (India)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9409999999999999</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.07199999999999995</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>01.07.2023 00:21 (Kyiv+Israel) 22:21 (UTC) 07:21 (Japan) 03:51 (India)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.885</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.05599999999999994</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
Fix for certf job (save and ext do not save job in section unfinished)
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
+++ b/ADtests/Resources/Extra files/RF LOAD RESULTS/SubmissionTime (2022).xlsx
@@ -1504,7 +1504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F113"/>
@@ -1770,6 +1770,52 @@
         <v>0.05599999999999994</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01.07.2023 01:45 (Kyiv+Israel) 23:45 (UTC) 08:45 (Japan) 05:15 (India)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.616</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01.07.2023 01:47 (Kyiv+Israel) 23:47 (UTC) 08:47 (Japan) 05:17 (India)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.201</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>

</xml_diff>